<commit_message>
:memo: Regras de negocio
Inserindo regras de negocio separadas
</commit_message>
<xml_diff>
--- a/Escritas em Gherkin/Gestão de teste_ Gherkin.xlsx
+++ b/Escritas em Gherkin/Gestão de teste_ Gherkin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FireII\Documents\Projetos\Plano_de_test_Site-----Matematica_da_agua\Escritas em Gherkin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA75EED-6563-4531-AB95-749EEC9042D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5079EC0-FDDA-4110-AE19-A015C812B674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Realizar o Acesso ao site" sheetId="1" r:id="rId1"/>
@@ -451,21 +451,21 @@
     <t>Não teve nenhuma ação</t>
   </si>
   <si>
-    <t xml:space="preserve">DADO que ao olocar o " Peso "
+    <t>ENTÃO  vou obter valores de ml e litros de água</t>
+  </si>
+  <si>
+    <t>Mensagem na tela: O resultado é igual a 3500 mL / 3.5 Litros</t>
+  </si>
+  <si>
+    <t>O site precisará estar disponivel e realizar diversas contas e os campos juntamente com botões devem estar conforme a proposta</t>
+  </si>
+  <si>
+    <t>Foi possível digitar qualquer letra no campo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DADO que ao colocar o " Peso "
 QUANDO ele for igual a 100kg
 E clicar em calcular </t>
-  </si>
-  <si>
-    <t>ENTÃO  vou obter valores de ml e litros de água</t>
-  </si>
-  <si>
-    <t>Mensagem na tela: O resultado é igual a 3500 mL / 3.5 Litros</t>
-  </si>
-  <si>
-    <t>O site precisará estar disponivel e realizar diversas contas e os campos juntamente com botões devem estar conforme a proposta</t>
-  </si>
-  <si>
-    <t>Foi possível digitar qualquer letra no campo</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -640,9 +640,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -668,6 +665,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,7 +894,9 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -961,11 +969,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>1</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="19" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -974,15 +982,15 @@
       <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -991,7 +999,7 @@
       <c r="D14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1009,7 +1017,7 @@
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
+      <c r="A20" s="9"/>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1018,7 +1026,7 @@
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2015,15 +2023,15 @@
   </sheetPr>
   <dimension ref="A4:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="64.28515625" customWidth="1"/>
-    <col min="2" max="2" width="68.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="2" max="2" width="77" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" customWidth="1"/>
     <col min="4" max="4" width="73.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2084,46 +2092,46 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>1</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>2</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="17" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="16" t="s">
+      <c r="D15" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>3</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="17" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -2132,15 +2140,15 @@
       <c r="D16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>4</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="18" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -2149,15 +2157,15 @@
       <c r="D17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="17" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -2166,7 +2174,7 @@
       <c r="D18" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2200,10 +2208,10 @@
     </row>
     <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
-      <c r="B29" s="17"/>
+      <c r="B29" s="16"/>
     </row>
     <row r="33" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D33" s="17"/>
+      <c r="D33" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2218,13 +2226,15 @@
   </sheetPr>
   <dimension ref="A4:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="64.28515625" customWidth="1"/>
     <col min="2" max="2" width="68.7109375" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="3" max="3" width="64" customWidth="1"/>
     <col min="4" max="4" width="58.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2285,11 +2295,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>1</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="18" t="s">
         <v>51</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -2298,15 +2308,15 @@
       <c r="D14" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>2</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="17" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -2315,59 +2325,59 @@
       <c r="D15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>3</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>58</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="9" t="s">
+      <c r="E16" s="9"/>
+      <c r="F16" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>4</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2378,7 +2388,7 @@
     </row>
     <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>